<commit_message>
Added new female ITT data
</commit_message>
<xml_diff>
--- a/Mouse Data/Liver AMPK Ketogenic Diet/All Figures/ITT/ITT 19-06-19.xlsx
+++ b/Mouse Data/Liver AMPK Ketogenic Diet/All Figures/ITT/ITT 19-06-19.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27907"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/BridgesLab/Kistler/AMPK KO/ITT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D02098-C9D6-A749-81F5-C451D24BAEC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" xr2:uid="{77BE3D11-62FB-7B43-8CA9-48B419828AE7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29460" windowHeight="17240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="20">
   <si>
     <t>Group</t>
   </si>
@@ -91,7 +96,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -470,11 +475,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29522801-309F-BD41-A320-875A1F4DB8ED}">
-  <dimension ref="A1:L81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="L91" sqref="L91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -915,247 +920,269 @@
       <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+      <c r="A13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1">
+        <v>193</v>
+      </c>
+      <c r="C13" s="2">
+        <v>145</v>
+      </c>
+      <c r="D13" s="2">
+        <v>139</v>
+      </c>
+      <c r="E13" s="2">
+        <v>128</v>
+      </c>
+      <c r="F13" s="2">
+        <v>102</v>
+      </c>
+      <c r="G13" s="2">
+        <v>120</v>
+      </c>
+      <c r="H13" s="2">
+        <v>148</v>
+      </c>
+      <c r="I13" s="2">
+        <v>199</v>
+      </c>
+      <c r="J13" s="2">
+        <v>219</v>
+      </c>
+      <c r="K13" s="2">
+        <v>241</v>
+      </c>
       <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
+      <c r="A14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1">
+        <v>194</v>
+      </c>
+      <c r="C14" s="2">
+        <v>200</v>
+      </c>
+      <c r="D14" s="2">
+        <v>191</v>
+      </c>
+      <c r="E14" s="2">
+        <v>133</v>
+      </c>
+      <c r="F14" s="2">
+        <v>121</v>
+      </c>
+      <c r="G14" s="2">
+        <v>107</v>
+      </c>
+      <c r="H14" s="2">
+        <v>117</v>
+      </c>
+      <c r="I14" s="2">
+        <v>142</v>
+      </c>
+      <c r="J14" s="2">
+        <v>148</v>
+      </c>
+      <c r="K14" s="2">
+        <v>170</v>
+      </c>
       <c r="L14" s="6"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B15" s="1">
-        <v>8191</v>
+        <v>855</v>
       </c>
       <c r="C15" s="2">
-        <v>135</v>
+        <v>162</v>
       </c>
       <c r="D15" s="2">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="E15" s="2">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="F15" s="2">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="G15" s="2">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H15" s="2">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="I15" s="2">
-        <v>78</v>
+        <v>159</v>
       </c>
       <c r="J15" s="2">
-        <v>82</v>
+        <v>154</v>
       </c>
       <c r="K15" s="2">
-        <v>90</v>
+        <v>172</v>
       </c>
       <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" s="1">
-        <v>8192</v>
+        <v>856</v>
       </c>
       <c r="C16" s="2">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="D16" s="2">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E16" s="2">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="F16" s="2">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="G16" s="2">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="H16" s="2">
-        <v>67</v>
+        <v>111</v>
       </c>
       <c r="I16" s="2">
-        <v>88</v>
+        <v>141</v>
       </c>
       <c r="J16" s="2">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="K16" s="2">
-        <v>108</v>
+        <v>130</v>
       </c>
       <c r="L16" s="6"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" s="1">
-        <v>8193</v>
+        <v>857</v>
       </c>
       <c r="C17" s="2">
-        <v>138</v>
+        <v>185</v>
       </c>
       <c r="D17" s="2">
-        <v>73</v>
+        <v>154</v>
       </c>
       <c r="E17" s="2">
-        <v>56</v>
+        <v>141</v>
       </c>
       <c r="F17" s="2">
-        <v>29</v>
+        <v>123</v>
       </c>
       <c r="G17" s="2">
-        <v>33</v>
+        <v>145</v>
       </c>
       <c r="H17" s="2">
-        <v>34</v>
+        <v>169</v>
       </c>
       <c r="I17" s="2">
-        <v>41</v>
+        <v>181</v>
       </c>
       <c r="J17" s="2">
-        <v>53</v>
+        <v>199</v>
       </c>
       <c r="K17" s="2">
-        <v>68</v>
+        <v>200</v>
       </c>
       <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B18" s="1">
-        <v>8194</v>
+        <v>883</v>
       </c>
       <c r="C18" s="2">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="D18" s="2">
-        <v>109</v>
+        <v>187</v>
       </c>
       <c r="E18" s="2">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F18" s="2">
-        <v>98</v>
+        <v>136</v>
       </c>
       <c r="G18" s="2">
-        <v>82</v>
+        <v>161</v>
       </c>
       <c r="H18" s="2">
-        <v>87</v>
+        <v>164</v>
       </c>
       <c r="I18" s="2">
-        <v>85</v>
+        <v>224</v>
       </c>
       <c r="J18" s="2">
-        <v>88</v>
+        <v>190</v>
       </c>
       <c r="K18" s="2">
-        <v>93</v>
+        <v>187</v>
       </c>
       <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" s="1">
-        <v>8556</v>
+        <v>884</v>
       </c>
       <c r="C19" s="2">
-        <v>131</v>
+        <v>168</v>
       </c>
       <c r="D19" s="2">
-        <v>116</v>
+        <v>248</v>
       </c>
       <c r="E19" s="2">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F19" s="2">
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="G19" s="2">
-        <v>136</v>
+        <v>217</v>
       </c>
       <c r="H19" s="2">
-        <v>145</v>
+        <v>233</v>
       </c>
       <c r="I19" s="2">
-        <v>154</v>
+        <v>230</v>
       </c>
       <c r="J19" s="2">
-        <v>165</v>
+        <v>239</v>
       </c>
       <c r="K19" s="2">
-        <v>153</v>
+        <v>246</v>
       </c>
       <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="1">
-        <v>8557</v>
-      </c>
-      <c r="C20" s="2">
-        <v>229</v>
-      </c>
-      <c r="D20" s="2">
-        <v>155</v>
-      </c>
-      <c r="E20" s="2">
-        <v>144</v>
-      </c>
-      <c r="F20" s="2">
-        <v>141</v>
-      </c>
-      <c r="G20" s="2">
-        <v>129</v>
-      </c>
-      <c r="H20" s="2">
-        <v>144</v>
-      </c>
-      <c r="I20" s="2">
-        <v>148</v>
-      </c>
-      <c r="J20" s="2">
-        <v>125</v>
-      </c>
-      <c r="K20" s="2">
-        <v>137</v>
-      </c>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
       <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -1163,34 +1190,34 @@
         <v>2</v>
       </c>
       <c r="B21" s="1">
-        <v>8559</v>
+        <v>8191</v>
       </c>
       <c r="C21" s="2">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="D21" s="2">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E21" s="2">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="F21" s="2">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="G21" s="2">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="H21" s="2">
-        <v>135</v>
+        <v>92</v>
       </c>
       <c r="I21" s="2">
-        <v>152</v>
+        <v>78</v>
       </c>
       <c r="J21" s="2">
-        <v>130</v>
+        <v>82</v>
       </c>
       <c r="K21" s="2">
-        <v>147</v>
+        <v>90</v>
       </c>
       <c r="L21" s="6"/>
     </row>
@@ -1199,31 +1226,31 @@
         <v>2</v>
       </c>
       <c r="B22" s="1">
-        <v>8786</v>
+        <v>8192</v>
       </c>
       <c r="C22" s="2">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="D22" s="2">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="E22" s="2">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="F22" s="2">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G22" s="2">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H22" s="2">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="I22" s="2">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="J22" s="2">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="K22" s="2">
         <v>108</v>
@@ -1231,261 +1258,261 @@
       <c r="L22" s="6"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
+      <c r="A23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1">
+        <v>8193</v>
+      </c>
+      <c r="C23" s="2">
+        <v>138</v>
+      </c>
+      <c r="D23" s="2">
+        <v>73</v>
+      </c>
+      <c r="E23" s="2">
+        <v>56</v>
+      </c>
+      <c r="F23" s="2">
+        <v>29</v>
+      </c>
+      <c r="G23" s="2">
+        <v>33</v>
+      </c>
+      <c r="H23" s="2">
+        <v>34</v>
+      </c>
+      <c r="I23" s="2">
+        <v>41</v>
+      </c>
+      <c r="J23" s="2">
+        <v>53</v>
+      </c>
+      <c r="K23" s="2">
+        <v>68</v>
+      </c>
       <c r="L23" s="6"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
+      <c r="A24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="1">
+        <v>8194</v>
+      </c>
+      <c r="C24" s="2">
+        <v>151</v>
+      </c>
+      <c r="D24" s="2">
+        <v>109</v>
+      </c>
+      <c r="E24" s="2">
+        <v>108</v>
+      </c>
+      <c r="F24" s="2">
+        <v>98</v>
+      </c>
+      <c r="G24" s="2">
+        <v>82</v>
+      </c>
+      <c r="H24" s="2">
+        <v>87</v>
+      </c>
+      <c r="I24" s="2">
+        <v>85</v>
+      </c>
+      <c r="J24" s="2">
+        <v>88</v>
+      </c>
+      <c r="K24" s="2">
+        <v>93</v>
+      </c>
       <c r="L24" s="6"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
+      <c r="A25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1">
+        <v>8556</v>
+      </c>
+      <c r="C25" s="2">
+        <v>131</v>
+      </c>
+      <c r="D25" s="2">
+        <v>116</v>
+      </c>
+      <c r="E25" s="2">
+        <v>115</v>
+      </c>
+      <c r="F25" s="2">
+        <v>132</v>
+      </c>
+      <c r="G25" s="2">
+        <v>136</v>
+      </c>
+      <c r="H25" s="2">
+        <v>145</v>
+      </c>
+      <c r="I25" s="2">
+        <v>154</v>
+      </c>
+      <c r="J25" s="2">
+        <v>165</v>
+      </c>
+      <c r="K25" s="2">
+        <v>153</v>
+      </c>
       <c r="L25" s="6"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B26" s="1">
-        <v>8265</v>
+        <v>8557</v>
       </c>
       <c r="C26" s="2">
-        <v>138</v>
+        <v>229</v>
       </c>
       <c r="D26" s="2">
-        <v>113</v>
+        <v>155</v>
       </c>
       <c r="E26" s="2">
-        <v>77</v>
+        <v>144</v>
       </c>
       <c r="F26" s="2">
-        <v>48</v>
+        <v>141</v>
       </c>
       <c r="G26" s="2">
-        <v>36</v>
+        <v>129</v>
       </c>
       <c r="H26" s="2">
-        <v>31</v>
+        <v>144</v>
       </c>
       <c r="I26" s="2">
-        <v>88</v>
+        <v>148</v>
       </c>
       <c r="J26" s="2">
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="K26" s="2">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="L26" s="6"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B27" s="1">
-        <v>8475</v>
+        <v>8559</v>
       </c>
       <c r="C27" s="2">
-        <v>134</v>
+        <v>164</v>
       </c>
       <c r="D27" s="2">
-        <v>99</v>
+        <v>135</v>
       </c>
       <c r="E27" s="2">
-        <v>86</v>
+        <v>124</v>
       </c>
       <c r="F27" s="2">
-        <v>59</v>
+        <v>130</v>
       </c>
       <c r="G27" s="2">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="H27" s="2">
-        <v>60</v>
+        <v>135</v>
       </c>
       <c r="I27" s="2">
-        <v>88</v>
+        <v>152</v>
       </c>
       <c r="J27" s="2">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="K27" s="2">
-        <v>99</v>
+        <v>147</v>
       </c>
       <c r="L27" s="6"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B28" s="1">
-        <v>8476</v>
+        <v>8786</v>
       </c>
       <c r="C28" s="2">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D28" s="2">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="E28" s="2">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="F28" s="2">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="G28" s="2">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="H28" s="2">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="I28" s="2">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="J28" s="2">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="K28" s="2">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="L28" s="6"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="1">
-        <v>8477</v>
-      </c>
-      <c r="C29" s="2">
-        <v>173</v>
-      </c>
-      <c r="D29" s="2">
-        <v>104</v>
-      </c>
-      <c r="E29" s="2">
-        <v>103</v>
-      </c>
-      <c r="F29" s="2">
-        <v>66</v>
-      </c>
-      <c r="G29" s="2">
-        <v>47</v>
-      </c>
-      <c r="H29" s="2">
-        <v>65</v>
-      </c>
-      <c r="I29" s="2">
-        <v>96</v>
-      </c>
-      <c r="J29" s="2">
-        <v>106</v>
-      </c>
-      <c r="K29" s="2">
-        <v>121</v>
-      </c>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
       <c r="L29" s="6"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B30" s="1">
-        <v>8564</v>
-      </c>
-      <c r="C30" s="2">
-        <v>129</v>
-      </c>
-      <c r="D30" s="2">
-        <v>147</v>
-      </c>
-      <c r="E30" s="2">
-        <v>107</v>
-      </c>
-      <c r="F30" s="2">
-        <v>153</v>
-      </c>
-      <c r="G30" s="2">
-        <v>117</v>
-      </c>
-      <c r="H30" s="2">
-        <v>147</v>
-      </c>
-      <c r="I30" s="2">
-        <v>140</v>
-      </c>
-      <c r="J30" s="2">
-        <v>137</v>
-      </c>
-      <c r="K30" s="2">
-        <v>130</v>
-      </c>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
       <c r="L30" s="6"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31" s="1">
-        <v>8565</v>
-      </c>
-      <c r="C31" s="2">
-        <v>150</v>
-      </c>
-      <c r="D31" s="2">
-        <v>107</v>
-      </c>
-      <c r="E31" s="2">
-        <v>107</v>
-      </c>
-      <c r="F31" s="2">
-        <v>168</v>
-      </c>
-      <c r="G31" s="2">
-        <v>109</v>
-      </c>
-      <c r="H31" s="2">
-        <v>121</v>
-      </c>
-      <c r="I31" s="2">
-        <v>120</v>
-      </c>
-      <c r="J31" s="2">
-        <v>122</v>
-      </c>
-      <c r="K31" s="2">
-        <v>120</v>
-      </c>
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
       <c r="L31" s="6"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
@@ -1493,1559 +1520,2252 @@
         <v>3</v>
       </c>
       <c r="B32" s="1">
-        <v>8566</v>
+        <v>8265</v>
       </c>
       <c r="C32" s="2">
+        <v>138</v>
+      </c>
+      <c r="D32" s="2">
         <v>113</v>
       </c>
-      <c r="D32" s="2">
-        <v>73</v>
-      </c>
       <c r="E32" s="2">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F32" s="2">
-        <v>108</v>
+        <v>48</v>
       </c>
       <c r="G32" s="2">
-        <v>124</v>
+        <v>36</v>
       </c>
       <c r="H32" s="2">
-        <v>135</v>
+        <v>31</v>
       </c>
       <c r="I32" s="2">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="J32" s="2">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="K32" s="2">
-        <v>101</v>
+        <v>143</v>
       </c>
       <c r="L32" s="6"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
+      <c r="A33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="1">
+        <v>8475</v>
+      </c>
+      <c r="C33" s="2">
+        <v>134</v>
+      </c>
+      <c r="D33" s="2">
+        <v>99</v>
+      </c>
+      <c r="E33" s="2">
+        <v>86</v>
+      </c>
+      <c r="F33" s="2">
+        <v>59</v>
+      </c>
+      <c r="G33" s="2">
+        <v>51</v>
+      </c>
+      <c r="H33" s="2">
+        <v>60</v>
+      </c>
+      <c r="I33" s="2">
+        <v>88</v>
+      </c>
+      <c r="J33" s="2">
+        <v>98</v>
+      </c>
+      <c r="K33" s="2">
+        <v>99</v>
+      </c>
       <c r="L33" s="6"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B34" s="1">
-        <v>8286</v>
+        <v>8476</v>
       </c>
       <c r="C34" s="2">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="D34" s="2">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="E34" s="2">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="F34" s="2">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="G34" s="2">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="H34" s="2">
-        <v>143</v>
+        <v>54</v>
       </c>
       <c r="I34" s="2">
-        <v>174</v>
+        <v>72</v>
       </c>
       <c r="J34" s="2">
-        <v>236</v>
+        <v>86</v>
       </c>
       <c r="K34" s="2">
-        <v>234</v>
+        <v>95</v>
       </c>
       <c r="L34" s="6"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B35" s="1">
-        <v>8287</v>
+        <v>8477</v>
       </c>
       <c r="C35" s="2">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="D35" s="2">
-        <v>141</v>
+        <v>104</v>
       </c>
       <c r="E35" s="2">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F35" s="2">
+        <v>66</v>
+      </c>
+      <c r="G35" s="2">
+        <v>47</v>
+      </c>
+      <c r="H35" s="2">
+        <v>65</v>
+      </c>
+      <c r="I35" s="2">
+        <v>96</v>
+      </c>
+      <c r="J35" s="2">
+        <v>106</v>
+      </c>
+      <c r="K35" s="2">
         <v>121</v>
-      </c>
-      <c r="G35" s="2">
-        <v>165</v>
-      </c>
-      <c r="H35" s="2">
-        <v>215</v>
-      </c>
-      <c r="I35" s="2">
-        <v>246</v>
-      </c>
-      <c r="J35" s="2">
-        <v>249</v>
-      </c>
-      <c r="K35" s="2">
-        <v>271</v>
       </c>
       <c r="L35" s="6"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B36" s="1">
-        <v>8288</v>
+        <v>8564</v>
       </c>
       <c r="C36" s="2">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="D36" s="2">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="E36" s="2">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="F36" s="2">
-        <v>78</v>
+        <v>153</v>
       </c>
       <c r="G36" s="2">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="H36" s="2">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="I36" s="2">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="J36" s="2">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="K36" s="2">
-        <v>183</v>
+        <v>130</v>
       </c>
       <c r="L36" s="6"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B37" s="1">
-        <v>8289</v>
+        <v>8565</v>
       </c>
       <c r="C37" s="2">
-        <v>181</v>
+        <v>150</v>
       </c>
       <c r="D37" s="2">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="E37" s="2">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="F37" s="2">
-        <v>103</v>
+        <v>168</v>
       </c>
       <c r="G37" s="2">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="H37" s="2">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="I37" s="2">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="J37" s="2">
-        <v>196</v>
+        <v>122</v>
       </c>
       <c r="K37" s="2">
-        <v>224</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="L37" s="6"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B38" s="1">
-        <v>8290</v>
+        <v>8566</v>
       </c>
       <c r="C38" s="2">
-        <v>222</v>
+        <v>113</v>
       </c>
       <c r="D38" s="2">
-        <v>126</v>
+        <v>73</v>
       </c>
       <c r="E38" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="F38" s="2">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="G38" s="2">
-        <v>86</v>
+        <v>124</v>
       </c>
       <c r="H38" s="2">
-        <v>99</v>
+        <v>135</v>
       </c>
       <c r="I38" s="2">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="J38" s="2">
-        <v>157</v>
+        <v>105</v>
       </c>
       <c r="K38" s="2">
-        <v>174</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="L38" s="6"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" s="1">
-        <v>8713</v>
-      </c>
-      <c r="C39" s="2">
-        <v>184</v>
-      </c>
-      <c r="D39" s="2">
-        <v>228</v>
-      </c>
-      <c r="E39" s="2">
-        <v>102</v>
-      </c>
-      <c r="F39" s="2">
-        <v>95</v>
-      </c>
-      <c r="G39" s="2">
-        <v>115</v>
-      </c>
-      <c r="H39" s="2">
-        <v>101</v>
-      </c>
-      <c r="I39" s="2">
-        <v>147</v>
-      </c>
-      <c r="J39" s="2">
-        <v>161</v>
-      </c>
-      <c r="K39" s="2">
-        <v>200</v>
-      </c>
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="6"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B40" s="1">
-        <v>8714</v>
+        <v>8286</v>
       </c>
       <c r="C40" s="2">
-        <v>210</v>
+        <v>175</v>
       </c>
       <c r="D40" s="2">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="E40" s="2">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F40" s="2">
-        <v>120</v>
+        <v>82</v>
       </c>
       <c r="G40" s="2">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="H40" s="2">
-        <v>82</v>
+        <v>143</v>
       </c>
       <c r="I40" s="2">
-        <v>108</v>
+        <v>174</v>
       </c>
       <c r="J40" s="2">
-        <v>126</v>
+        <v>236</v>
       </c>
       <c r="K40" s="2">
-        <v>136</v>
-      </c>
-      <c r="L40" s="2"/>
+        <v>234</v>
+      </c>
+      <c r="L40" s="6"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B41" s="1">
-        <v>8720</v>
+        <v>8287</v>
       </c>
       <c r="C41" s="2">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="D41" s="2">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="E41" s="2">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F41" s="2">
-        <v>86</v>
+        <v>121</v>
       </c>
       <c r="G41" s="2">
-        <v>79</v>
+        <v>165</v>
       </c>
       <c r="H41" s="2">
-        <v>74</v>
+        <v>215</v>
       </c>
       <c r="I41" s="2">
-        <v>117</v>
+        <v>246</v>
       </c>
       <c r="J41" s="2">
-        <v>131</v>
+        <v>249</v>
       </c>
       <c r="K41" s="2">
-        <v>155</v>
-      </c>
+        <v>271</v>
+      </c>
+      <c r="L41" s="6"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
+      <c r="A42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="1">
+        <v>8288</v>
+      </c>
+      <c r="C42" s="2">
+        <v>159</v>
+      </c>
+      <c r="D42" s="2">
+        <v>129</v>
+      </c>
+      <c r="E42" s="2">
+        <v>81</v>
+      </c>
+      <c r="F42" s="2">
+        <v>78</v>
+      </c>
+      <c r="G42" s="2">
+        <v>90</v>
+      </c>
+      <c r="H42" s="2">
+        <v>116</v>
+      </c>
+      <c r="I42" s="2">
+        <v>133</v>
+      </c>
+      <c r="J42" s="2">
+        <v>171</v>
+      </c>
+      <c r="K42" s="2">
+        <v>183</v>
+      </c>
+      <c r="L42" s="6"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
+      <c r="A43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="1">
+        <v>8289</v>
+      </c>
+      <c r="C43" s="2">
+        <v>181</v>
+      </c>
+      <c r="D43" s="2">
+        <v>119</v>
+      </c>
+      <c r="E43" s="2">
+        <v>102</v>
+      </c>
+      <c r="F43" s="2">
+        <v>103</v>
+      </c>
+      <c r="G43" s="2">
+        <v>101</v>
+      </c>
+      <c r="H43" s="2">
+        <v>110</v>
+      </c>
+      <c r="I43" s="2">
+        <v>160</v>
+      </c>
+      <c r="J43" s="2">
+        <v>196</v>
+      </c>
+      <c r="K43" s="2">
+        <v>224</v>
+      </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B44" s="1">
-        <v>8187</v>
+        <v>8290</v>
       </c>
       <c r="C44" s="2">
-        <v>188</v>
+        <v>222</v>
       </c>
       <c r="D44" s="2">
-        <v>164</v>
+        <v>126</v>
       </c>
       <c r="E44" s="2">
-        <v>115</v>
+        <v>79</v>
       </c>
       <c r="F44" s="2">
+        <v>80</v>
+      </c>
+      <c r="G44" s="2">
+        <v>86</v>
+      </c>
+      <c r="H44" s="2">
         <v>99</v>
       </c>
-      <c r="G44" s="2">
-        <v>155</v>
-      </c>
-      <c r="H44" s="2">
-        <v>197</v>
-      </c>
       <c r="I44" s="2">
-        <v>233</v>
+        <v>121</v>
       </c>
       <c r="J44" s="2">
-        <v>225</v>
+        <v>157</v>
       </c>
       <c r="K44" s="2">
-        <v>238</v>
+        <v>174</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B45" s="1">
-        <v>8188</v>
+        <v>8713</v>
       </c>
       <c r="C45" s="2">
+        <v>184</v>
+      </c>
+      <c r="D45" s="2">
+        <v>228</v>
+      </c>
+      <c r="E45" s="2">
+        <v>102</v>
+      </c>
+      <c r="F45" s="2">
+        <v>95</v>
+      </c>
+      <c r="G45" s="2">
+        <v>115</v>
+      </c>
+      <c r="H45" s="2">
+        <v>101</v>
+      </c>
+      <c r="I45" s="2">
+        <v>147</v>
+      </c>
+      <c r="J45" s="2">
+        <v>161</v>
+      </c>
+      <c r="K45" s="2">
         <v>200</v>
-      </c>
-      <c r="D45" s="2">
-        <v>196</v>
-      </c>
-      <c r="E45" s="2">
-        <v>175</v>
-      </c>
-      <c r="F45" s="2">
-        <v>174</v>
-      </c>
-      <c r="G45" s="2">
-        <v>180</v>
-      </c>
-      <c r="H45" s="2">
-        <v>187</v>
-      </c>
-      <c r="I45" s="2">
-        <v>202</v>
-      </c>
-      <c r="J45" s="2">
-        <v>178</v>
-      </c>
-      <c r="K45" s="2">
-        <v>218</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B46" s="1">
-        <v>8190</v>
+        <v>8714</v>
       </c>
       <c r="C46" s="2">
-        <v>231</v>
+        <v>210</v>
       </c>
       <c r="D46" s="2">
-        <v>195</v>
+        <v>134</v>
       </c>
       <c r="E46" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F46" s="2">
-        <v>91</v>
+        <v>120</v>
       </c>
       <c r="G46" s="2">
-        <v>113</v>
+        <v>88</v>
       </c>
       <c r="H46" s="2">
-        <v>141</v>
+        <v>82</v>
       </c>
       <c r="I46" s="2">
-        <v>180</v>
+        <v>108</v>
       </c>
       <c r="J46" s="2">
-        <v>199</v>
+        <v>126</v>
       </c>
       <c r="K46" s="2">
-        <v>224</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="L46" s="2"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B47" s="1">
-        <v>8473</v>
+        <v>8720</v>
       </c>
       <c r="C47" s="2">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D47" s="2">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E47" s="2">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="F47" s="2">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="G47" s="2">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="H47" s="2">
-        <v>140</v>
+        <v>74</v>
       </c>
       <c r="I47" s="2">
-        <v>213</v>
+        <v>117</v>
       </c>
       <c r="J47" s="2">
-        <v>227</v>
+        <v>131</v>
       </c>
       <c r="K47" s="2">
-        <v>234</v>
+        <v>155</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="1">
+        <v>195</v>
+      </c>
+      <c r="C48" s="2">
+        <v>114</v>
+      </c>
+      <c r="D48" s="2">
+        <v>113</v>
+      </c>
+      <c r="E48" s="2">
+        <v>90</v>
+      </c>
+      <c r="F48" s="2">
+        <v>123</v>
+      </c>
+      <c r="G48" s="2">
+        <v>193</v>
+      </c>
+      <c r="H48" s="2">
+        <v>309</v>
+      </c>
+      <c r="I48" s="2">
+        <v>415</v>
+      </c>
+      <c r="J48" s="2">
+        <v>430</v>
+      </c>
+      <c r="K48" s="2">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="1">
+        <v>196</v>
+      </c>
+      <c r="C49" s="2">
+        <v>129</v>
+      </c>
+      <c r="D49" s="2">
+        <v>124</v>
+      </c>
+      <c r="E49" s="2">
+        <v>106</v>
+      </c>
+      <c r="F49" s="2">
+        <v>130</v>
+      </c>
+      <c r="G49" s="2">
+        <v>197</v>
+      </c>
+      <c r="H49" s="2">
+        <v>305</v>
+      </c>
+      <c r="I49" s="2">
+        <v>298</v>
+      </c>
+      <c r="J49" s="2">
+        <v>280</v>
+      </c>
+      <c r="K49" s="2">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" s="1">
+        <v>197</v>
+      </c>
+      <c r="C50" s="2">
+        <v>141</v>
+      </c>
+      <c r="D50" s="2">
+        <v>132</v>
+      </c>
+      <c r="E50" s="2">
+        <v>117</v>
+      </c>
+      <c r="F50" s="2">
+        <v>103</v>
+      </c>
+      <c r="G50" s="2">
+        <v>129</v>
+      </c>
+      <c r="H50" s="2">
+        <v>194</v>
+      </c>
+      <c r="I50" s="2">
+        <v>208</v>
+      </c>
+      <c r="J50" s="2">
+        <v>199</v>
+      </c>
+      <c r="K50" s="2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="1">
+        <v>858</v>
+      </c>
+      <c r="C51" s="2">
+        <v>208</v>
+      </c>
+      <c r="D51" s="2">
+        <v>149</v>
+      </c>
+      <c r="E51" s="2">
+        <v>99</v>
+      </c>
+      <c r="F51" s="2">
+        <v>122</v>
+      </c>
+      <c r="G51" s="2">
+        <v>162</v>
+      </c>
+      <c r="H51" s="2">
+        <v>200</v>
+      </c>
+      <c r="I51" s="2">
+        <v>198</v>
+      </c>
+      <c r="J51" s="2">
+        <v>187</v>
+      </c>
+      <c r="K51" s="2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="1">
+        <v>859</v>
+      </c>
+      <c r="C52" s="2">
+        <v>186</v>
+      </c>
+      <c r="D52" s="2">
+        <v>154</v>
+      </c>
+      <c r="E52" s="2">
+        <v>99</v>
+      </c>
+      <c r="F52" s="2">
+        <v>132</v>
+      </c>
+      <c r="G52" s="2">
+        <v>178</v>
+      </c>
+      <c r="H52" s="2">
+        <v>232</v>
+      </c>
+      <c r="I52" s="2">
+        <v>203</v>
+      </c>
+      <c r="J52" s="2">
+        <v>189</v>
+      </c>
+      <c r="K52" s="2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" s="1">
+        <v>860</v>
+      </c>
+      <c r="C53" s="2">
+        <v>211</v>
+      </c>
+      <c r="D53" s="2">
+        <v>181</v>
+      </c>
+      <c r="E53" s="2">
+        <v>112</v>
+      </c>
+      <c r="F53" s="2">
+        <v>147</v>
+      </c>
+      <c r="G53" s="2">
+        <v>149</v>
+      </c>
+      <c r="H53" s="2">
+        <v>174</v>
+      </c>
+      <c r="I53" s="2">
+        <v>196</v>
+      </c>
+      <c r="J53" s="2">
+        <v>181</v>
+      </c>
+      <c r="K53" s="2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" s="1">
+        <v>885</v>
+      </c>
+      <c r="C54" s="2">
+        <v>127</v>
+      </c>
+      <c r="D54" s="2">
+        <v>116</v>
+      </c>
+      <c r="E54" s="2">
+        <v>92</v>
+      </c>
+      <c r="F54" s="2">
+        <v>104</v>
+      </c>
+      <c r="G54" s="2">
+        <v>141</v>
+      </c>
+      <c r="H54" s="2">
+        <v>180</v>
+      </c>
+      <c r="I54" s="2">
+        <v>199</v>
+      </c>
+      <c r="J54" s="2">
+        <v>183</v>
+      </c>
+      <c r="K54" s="2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" s="1">
+        <v>886</v>
+      </c>
+      <c r="C55" s="2">
+        <v>129</v>
+      </c>
+      <c r="D55" s="2">
+        <v>163</v>
+      </c>
+      <c r="E55" s="2">
+        <v>117</v>
+      </c>
+      <c r="F55" s="2">
+        <v>144</v>
+      </c>
+      <c r="G55" s="2">
+        <v>186</v>
+      </c>
+      <c r="H55" s="2">
+        <v>246</v>
+      </c>
+      <c r="I55" s="2">
+        <v>315</v>
+      </c>
+      <c r="J55" s="2">
+        <v>285</v>
+      </c>
+      <c r="K55" s="2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="1">
+        <v>888</v>
+      </c>
+      <c r="C56" s="2">
+        <v>131</v>
+      </c>
+      <c r="D56" s="2">
+        <v>183</v>
+      </c>
+      <c r="E56" s="2">
+        <v>127</v>
+      </c>
+      <c r="F56" s="2">
+        <v>126</v>
+      </c>
+      <c r="G56" s="2">
+        <v>141</v>
+      </c>
+      <c r="H56" s="2">
+        <v>188</v>
+      </c>
+      <c r="I56" s="2">
+        <v>215</v>
+      </c>
+      <c r="J56" s="2">
+        <v>224</v>
+      </c>
+      <c r="K56" s="2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B58" s="1">
+        <v>8187</v>
+      </c>
+      <c r="C58" s="2">
+        <v>188</v>
+      </c>
+      <c r="D58" s="2">
+        <v>164</v>
+      </c>
+      <c r="E58" s="2">
+        <v>115</v>
+      </c>
+      <c r="F58" s="2">
+        <v>99</v>
+      </c>
+      <c r="G58" s="2">
+        <v>155</v>
+      </c>
+      <c r="H58" s="2">
+        <v>197</v>
+      </c>
+      <c r="I58" s="2">
+        <v>233</v>
+      </c>
+      <c r="J58" s="2">
+        <v>225</v>
+      </c>
+      <c r="K58" s="2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59" s="1">
+        <v>8188</v>
+      </c>
+      <c r="C59" s="2">
+        <v>200</v>
+      </c>
+      <c r="D59" s="2">
+        <v>196</v>
+      </c>
+      <c r="E59" s="2">
+        <v>175</v>
+      </c>
+      <c r="F59" s="2">
+        <v>174</v>
+      </c>
+      <c r="G59" s="2">
+        <v>180</v>
+      </c>
+      <c r="H59" s="2">
+        <v>187</v>
+      </c>
+      <c r="I59" s="2">
+        <v>202</v>
+      </c>
+      <c r="J59" s="2">
+        <v>178</v>
+      </c>
+      <c r="K59" s="2">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" s="1">
+        <v>8190</v>
+      </c>
+      <c r="C60" s="2">
+        <v>231</v>
+      </c>
+      <c r="D60" s="2">
+        <v>195</v>
+      </c>
+      <c r="E60" s="2">
+        <v>103</v>
+      </c>
+      <c r="F60" s="2">
+        <v>91</v>
+      </c>
+      <c r="G60" s="2">
+        <v>113</v>
+      </c>
+      <c r="H60" s="2">
+        <v>141</v>
+      </c>
+      <c r="I60" s="2">
+        <v>180</v>
+      </c>
+      <c r="J60" s="2">
+        <v>199</v>
+      </c>
+      <c r="K60" s="2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="1">
+        <v>8473</v>
+      </c>
+      <c r="C61" s="2">
+        <v>179</v>
+      </c>
+      <c r="D61" s="2">
+        <v>162</v>
+      </c>
+      <c r="E61" s="2">
+        <v>130</v>
+      </c>
+      <c r="F61" s="2">
+        <v>103</v>
+      </c>
+      <c r="G61" s="2">
+        <v>111</v>
+      </c>
+      <c r="H61" s="2">
+        <v>140</v>
+      </c>
+      <c r="I61" s="2">
+        <v>213</v>
+      </c>
+      <c r="J61" s="2">
+        <v>227</v>
+      </c>
+      <c r="K61" s="2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" s="1">
         <v>8474</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C62" s="2">
         <v>160</v>
       </c>
-      <c r="D48" s="2">
+      <c r="D62" s="2">
         <v>193</v>
       </c>
-      <c r="E48" s="2">
+      <c r="E62" s="2">
         <v>124</v>
       </c>
-      <c r="F48" s="2">
+      <c r="F62" s="2">
         <v>93</v>
       </c>
-      <c r="G48" s="2">
+      <c r="G62" s="2">
         <v>122</v>
       </c>
-      <c r="H48" s="2">
+      <c r="H62" s="2">
         <v>148</v>
       </c>
-      <c r="I48" s="2">
+      <c r="I62" s="2">
         <v>206</v>
       </c>
-      <c r="J48" s="2">
+      <c r="J62" s="2">
         <v>215</v>
       </c>
-      <c r="K48" s="2">
+      <c r="K62" s="2">
         <v>261</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B63" s="1">
         <v>8821</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C63" s="2">
         <v>153</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D63" s="2">
         <v>130</v>
       </c>
-      <c r="E49" s="2">
+      <c r="E63" s="2">
         <v>104</v>
       </c>
-      <c r="F49" s="2">
+      <c r="F63" s="2">
         <v>95</v>
       </c>
-      <c r="G49" s="2">
+      <c r="G63" s="2">
         <v>119</v>
       </c>
-      <c r="H49" s="2">
+      <c r="H63" s="2">
         <v>164</v>
       </c>
-      <c r="I49" s="2">
+      <c r="I63" s="2">
         <v>168</v>
       </c>
-      <c r="J49" s="2">
+      <c r="J63" s="2">
         <v>189</v>
       </c>
-      <c r="K49" s="2">
+      <c r="K63" s="2">
         <v>194</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B64" s="1">
         <v>8822</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C64" s="2">
         <v>131</v>
       </c>
-      <c r="D50" s="2">
+      <c r="D64" s="2">
         <v>127</v>
       </c>
-      <c r="E50" s="2">
+      <c r="E64" s="2">
         <v>84</v>
       </c>
-      <c r="F50" s="2">
+      <c r="F64" s="2">
         <v>86</v>
       </c>
-      <c r="G50" s="2">
+      <c r="G64" s="2">
         <v>107</v>
       </c>
-      <c r="H50" s="2">
+      <c r="H64" s="2">
         <v>122</v>
       </c>
-      <c r="I50" s="2">
+      <c r="I64" s="2">
         <v>121</v>
       </c>
-      <c r="J50" s="2">
+      <c r="J64" s="2">
         <v>147</v>
       </c>
-      <c r="K50" s="2">
+      <c r="K64" s="2">
         <v>148</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B65" s="1">
         <v>8823</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C65" s="2">
         <v>173</v>
       </c>
-      <c r="D51" s="2">
+      <c r="D65" s="2">
         <v>181</v>
       </c>
-      <c r="E51" s="2">
+      <c r="E65" s="2">
         <v>103</v>
       </c>
-      <c r="F51" s="2">
+      <c r="F65" s="2">
         <v>101</v>
       </c>
-      <c r="G51" s="2">
+      <c r="G65" s="2">
         <v>113</v>
       </c>
-      <c r="H51" s="2">
+      <c r="H65" s="2">
         <v>133</v>
       </c>
-      <c r="I51" s="2">
+      <c r="I65" s="2">
         <v>154</v>
       </c>
-      <c r="J51" s="2">
+      <c r="J65" s="2">
         <v>179</v>
       </c>
-      <c r="K51" s="2">
+      <c r="K65" s="2">
         <v>180</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B52" s="1">
-        <v>8824</v>
-      </c>
-      <c r="C52" s="2">
-        <v>157</v>
-      </c>
-      <c r="D52" s="2">
-        <v>165</v>
-      </c>
-      <c r="E52" s="2">
-        <v>101</v>
-      </c>
-      <c r="F52" s="2">
-        <v>98</v>
-      </c>
-      <c r="G52" s="2">
-        <v>142</v>
-      </c>
-      <c r="H52" s="2">
-        <v>159</v>
-      </c>
-      <c r="I52" s="2">
-        <v>205</v>
-      </c>
-      <c r="J52" s="2">
-        <v>202</v>
-      </c>
-      <c r="K52" s="2">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B54" s="1">
-        <v>8148</v>
-      </c>
-      <c r="C54" s="2">
-        <v>130</v>
-      </c>
-      <c r="D54" s="2">
-        <v>67</v>
-      </c>
-      <c r="E54" s="2">
-        <v>51</v>
-      </c>
-      <c r="F54" s="2">
-        <v>34</v>
-      </c>
-      <c r="G54" s="2">
-        <v>37</v>
-      </c>
-      <c r="H54" s="2">
-        <v>47</v>
-      </c>
-      <c r="I54" s="2">
-        <v>63</v>
-      </c>
-      <c r="J54" s="2">
-        <v>76</v>
-      </c>
-      <c r="K54" s="2">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B55" s="1">
-        <v>8149</v>
-      </c>
-      <c r="C55" s="2">
-        <v>157</v>
-      </c>
-      <c r="D55" s="2">
-        <v>84</v>
-      </c>
-      <c r="E55" s="2">
-        <v>99</v>
-      </c>
-      <c r="F55" s="2">
-        <v>88</v>
-      </c>
-      <c r="G55" s="2">
-        <v>105</v>
-      </c>
-      <c r="H55" s="2">
-        <v>105</v>
-      </c>
-      <c r="I55" s="2">
-        <v>122</v>
-      </c>
-      <c r="J55" s="2">
-        <v>130</v>
-      </c>
-      <c r="K55" s="2">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B56" s="1">
-        <v>8263</v>
-      </c>
-      <c r="C56" s="2">
-        <v>205</v>
-      </c>
-      <c r="D56" s="2">
-        <v>175</v>
-      </c>
-      <c r="E56" s="2">
-        <v>128</v>
-      </c>
-      <c r="F56" s="2">
-        <v>118</v>
-      </c>
-      <c r="G56" s="2">
-        <v>126</v>
-      </c>
-      <c r="H56" s="2">
-        <v>131</v>
-      </c>
-      <c r="I56" s="2">
-        <v>149</v>
-      </c>
-      <c r="J56" s="2">
-        <v>159</v>
-      </c>
-      <c r="K56" s="2">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B57" s="1">
-        <v>8457</v>
-      </c>
-      <c r="C57" s="2">
-        <v>151</v>
-      </c>
-      <c r="D57" s="2">
-        <v>103</v>
-      </c>
-      <c r="E57" s="2">
-        <v>120</v>
-      </c>
-      <c r="F57" s="2">
-        <v>94</v>
-      </c>
-      <c r="G57" s="2">
-        <v>108</v>
-      </c>
-      <c r="H57" s="2">
-        <v>104</v>
-      </c>
-      <c r="I57" s="2">
-        <v>147</v>
-      </c>
-      <c r="J57" s="2">
-        <v>177</v>
-      </c>
-      <c r="K57" s="2">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B58" s="1">
-        <v>8708</v>
-      </c>
-      <c r="C58" s="2">
-        <v>158</v>
-      </c>
-      <c r="D58" s="2">
-        <v>102</v>
-      </c>
-      <c r="E58" s="2">
-        <v>80</v>
-      </c>
-      <c r="F58" s="2">
-        <v>59</v>
-      </c>
-      <c r="G58" s="2">
-        <v>40</v>
-      </c>
-      <c r="H58" s="2">
-        <v>40</v>
-      </c>
-      <c r="I58" s="2">
-        <v>63</v>
-      </c>
-      <c r="J58" s="2">
-        <v>89</v>
-      </c>
-      <c r="K58" s="2">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B59" s="1">
-        <v>8709</v>
-      </c>
-      <c r="C59" s="2">
-        <v>138</v>
-      </c>
-      <c r="D59" s="2">
-        <v>91</v>
-      </c>
-      <c r="E59" s="2">
-        <v>98</v>
-      </c>
-      <c r="F59" s="2">
-        <v>85</v>
-      </c>
-      <c r="G59" s="2">
-        <v>76</v>
-      </c>
-      <c r="H59" s="2">
-        <v>67</v>
-      </c>
-      <c r="I59" s="2">
-        <v>85</v>
-      </c>
-      <c r="J59" s="2">
-        <v>91</v>
-      </c>
-      <c r="K59" s="2">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B60" s="1">
-        <v>8710</v>
-      </c>
-      <c r="C60" s="2">
-        <v>131</v>
-      </c>
-      <c r="D60" s="2">
-        <v>91</v>
-      </c>
-      <c r="E60" s="2">
-        <v>53</v>
-      </c>
-      <c r="F60" s="2">
-        <v>34</v>
-      </c>
-      <c r="G60" s="2">
-        <v>32</v>
-      </c>
-      <c r="H60" s="2">
-        <v>28</v>
-      </c>
-      <c r="I60" s="2">
-        <v>43</v>
-      </c>
-      <c r="J60" s="2">
-        <v>77</v>
-      </c>
-      <c r="K60" s="2">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B61" s="1">
-        <v>8711</v>
-      </c>
-      <c r="C61" s="2">
-        <v>162</v>
-      </c>
-      <c r="D61" s="2">
-        <v>89</v>
-      </c>
-      <c r="E61" s="2">
-        <v>49</v>
-      </c>
-      <c r="F61" s="2">
-        <v>28</v>
-      </c>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
-      <c r="J61" s="2"/>
-      <c r="K61" s="2"/>
-      <c r="L61" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B62" s="1">
-        <v>8712</v>
-      </c>
-      <c r="C62" s="2">
-        <v>158</v>
-      </c>
-      <c r="D62" s="2">
-        <v>113</v>
-      </c>
-      <c r="E62" s="2">
-        <v>92</v>
-      </c>
-      <c r="F62" s="2">
-        <v>85</v>
-      </c>
-      <c r="G62" s="2">
-        <v>66</v>
-      </c>
-      <c r="H62" s="2">
-        <v>63</v>
-      </c>
-      <c r="I62" s="2">
-        <v>78</v>
-      </c>
-      <c r="J62" s="2">
-        <v>92</v>
-      </c>
-      <c r="K62" s="2">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
-      <c r="K63" s="2"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
-      <c r="K64" s="2"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
-      <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
-      <c r="I65" s="2"/>
-      <c r="J65" s="2"/>
-      <c r="K65" s="2"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B66" s="1">
-        <v>8151</v>
+        <v>8824</v>
       </c>
       <c r="C66" s="2">
+        <v>157</v>
+      </c>
+      <c r="D66" s="2">
         <v>165</v>
       </c>
-      <c r="D66" s="2">
-        <v>131</v>
-      </c>
       <c r="E66" s="2">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F66" s="2">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="G66" s="2">
-        <v>91</v>
+        <v>142</v>
       </c>
       <c r="H66" s="2">
-        <v>103</v>
+        <v>159</v>
       </c>
       <c r="I66" s="2">
-        <v>143</v>
+        <v>205</v>
       </c>
       <c r="J66" s="2">
-        <v>158</v>
+        <v>202</v>
       </c>
       <c r="K66" s="2">
-        <v>180</v>
+        <v>209</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B67" s="1">
-        <v>8152</v>
+        <v>192</v>
       </c>
       <c r="C67" s="2">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D67" s="2">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="E67" s="2">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F67" s="2">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="G67" s="2">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="H67" s="2">
-        <v>195</v>
+        <v>138</v>
       </c>
       <c r="I67" s="2">
-        <v>223</v>
+        <v>162</v>
       </c>
       <c r="J67" s="2">
-        <v>227</v>
+        <v>170</v>
       </c>
       <c r="K67" s="2">
-        <v>236</v>
+        <v>184</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B68" s="1">
-        <v>8153</v>
+        <v>853</v>
       </c>
       <c r="C68" s="2">
-        <v>194</v>
+        <v>235</v>
       </c>
       <c r="D68" s="2">
+        <v>243</v>
+      </c>
+      <c r="E68" s="2">
+        <v>149</v>
+      </c>
+      <c r="F68" s="2">
+        <v>171</v>
+      </c>
+      <c r="G68" s="2">
+        <v>79</v>
+      </c>
+      <c r="H68" s="2">
         <v>193</v>
       </c>
-      <c r="E68" s="2">
-        <v>93</v>
-      </c>
-      <c r="F68" s="2">
-        <v>92</v>
-      </c>
-      <c r="G68" s="2">
-        <v>103</v>
-      </c>
-      <c r="H68" s="2">
-        <v>131</v>
-      </c>
       <c r="I68" s="2">
-        <v>159</v>
+        <v>182</v>
       </c>
       <c r="J68" s="2">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="K68" s="2">
-        <v>182</v>
+        <v>199</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B69" s="1">
-        <v>8154</v>
+        <v>854</v>
       </c>
       <c r="C69" s="2">
-        <v>165</v>
+        <v>268</v>
       </c>
       <c r="D69" s="2">
-        <v>128</v>
+        <v>243</v>
       </c>
       <c r="E69" s="2">
-        <v>92</v>
+        <v>154</v>
       </c>
       <c r="F69" s="2">
-        <v>80</v>
+        <v>147</v>
       </c>
       <c r="G69" s="2">
-        <v>112</v>
+        <v>182</v>
       </c>
       <c r="H69" s="2">
-        <v>142</v>
+        <v>234</v>
       </c>
       <c r="I69" s="2">
-        <v>155</v>
+        <v>266</v>
       </c>
       <c r="J69" s="2">
-        <v>192</v>
+        <v>283</v>
       </c>
       <c r="K69" s="2">
-        <v>181</v>
+        <v>296</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B70" s="1">
-        <v>8827</v>
-      </c>
-      <c r="C70" s="6">
-        <v>147</v>
-      </c>
-      <c r="D70" s="6">
-        <v>107</v>
-      </c>
-      <c r="E70" s="6">
-        <v>92</v>
-      </c>
-      <c r="F70" s="6">
-        <v>98</v>
-      </c>
-      <c r="G70" s="6">
-        <v>114</v>
-      </c>
-      <c r="H70" s="6">
-        <v>140</v>
-      </c>
-      <c r="I70" s="6">
-        <v>174</v>
-      </c>
-      <c r="J70" s="6">
-        <v>179</v>
-      </c>
-      <c r="K70" s="6">
-        <v>175</v>
-      </c>
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
+      <c r="K70" s="2"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B71" s="1">
-        <v>8828</v>
-      </c>
-      <c r="C71" s="6">
-        <v>122</v>
-      </c>
-      <c r="D71" s="6">
-        <v>71</v>
-      </c>
-      <c r="E71" s="6">
-        <v>91</v>
-      </c>
-      <c r="F71" s="6">
-        <v>86</v>
-      </c>
-      <c r="G71" s="6">
-        <v>118</v>
-      </c>
-      <c r="H71" s="6">
-        <v>136</v>
-      </c>
-      <c r="I71" s="6">
-        <v>182</v>
-      </c>
-      <c r="J71" s="6">
-        <v>219</v>
-      </c>
-      <c r="K71" s="6">
-        <v>228</v>
+        <v>8148</v>
+      </c>
+      <c r="C71" s="2">
+        <v>130</v>
+      </c>
+      <c r="D71" s="2">
+        <v>67</v>
+      </c>
+      <c r="E71" s="2">
+        <v>51</v>
+      </c>
+      <c r="F71" s="2">
+        <v>34</v>
+      </c>
+      <c r="G71" s="2">
+        <v>37</v>
+      </c>
+      <c r="H71" s="2">
+        <v>47</v>
+      </c>
+      <c r="I71" s="2">
+        <v>63</v>
+      </c>
+      <c r="J71" s="2">
+        <v>76</v>
+      </c>
+      <c r="K71" s="2">
+        <v>94</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B72" s="1">
-        <v>8829</v>
+        <v>8149</v>
       </c>
       <c r="C72" s="2">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D72" s="2">
-        <v>150</v>
+        <v>84</v>
       </c>
       <c r="E72" s="2">
+        <v>99</v>
+      </c>
+      <c r="F72" s="2">
+        <v>88</v>
+      </c>
+      <c r="G72" s="2">
+        <v>105</v>
+      </c>
+      <c r="H72" s="2">
+        <v>105</v>
+      </c>
+      <c r="I72" s="2">
+        <v>122</v>
+      </c>
+      <c r="J72" s="2">
+        <v>130</v>
+      </c>
+      <c r="K72" s="2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" s="1">
+        <v>8263</v>
+      </c>
+      <c r="C73" s="2">
+        <v>205</v>
+      </c>
+      <c r="D73" s="2">
+        <v>175</v>
+      </c>
+      <c r="E73" s="2">
+        <v>128</v>
+      </c>
+      <c r="F73" s="2">
+        <v>118</v>
+      </c>
+      <c r="G73" s="2">
+        <v>126</v>
+      </c>
+      <c r="H73" s="2">
+        <v>131</v>
+      </c>
+      <c r="I73" s="2">
+        <v>149</v>
+      </c>
+      <c r="J73" s="2">
+        <v>159</v>
+      </c>
+      <c r="K73" s="2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B74" s="1">
+        <v>8457</v>
+      </c>
+      <c r="C74" s="2">
+        <v>151</v>
+      </c>
+      <c r="D74" s="2">
         <v>103</v>
       </c>
-      <c r="F72" s="2">
-        <v>107</v>
-      </c>
-      <c r="G72" s="2">
-        <v>113</v>
-      </c>
-      <c r="H72" s="2">
-        <v>146</v>
-      </c>
-      <c r="I72" s="2">
-        <v>183</v>
-      </c>
-      <c r="J72" s="2">
+      <c r="E74" s="2">
+        <v>120</v>
+      </c>
+      <c r="F74" s="2">
+        <v>94</v>
+      </c>
+      <c r="G74" s="2">
+        <v>108</v>
+      </c>
+      <c r="H74" s="2">
+        <v>104</v>
+      </c>
+      <c r="I74" s="2">
+        <v>147</v>
+      </c>
+      <c r="J74" s="2">
+        <v>177</v>
+      </c>
+      <c r="K74" s="2">
         <v>196</v>
-      </c>
-      <c r="K72" s="2">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A74" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B74" s="7">
-        <v>8560</v>
-      </c>
-      <c r="C74" s="7">
-        <v>196</v>
-      </c>
-      <c r="D74" s="7">
-        <v>124</v>
-      </c>
-      <c r="E74" s="7">
-        <v>151</v>
-      </c>
-      <c r="F74" s="7">
-        <v>155</v>
-      </c>
-      <c r="G74" s="7">
-        <v>148</v>
-      </c>
-      <c r="H74" s="7">
-        <v>151</v>
-      </c>
-      <c r="I74" s="7">
-        <v>153</v>
-      </c>
-      <c r="J74" s="7">
-        <v>168</v>
-      </c>
-      <c r="K74" s="7">
-        <v>155</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B75" s="1">
-        <v>8347</v>
-      </c>
-      <c r="C75" s="7">
-        <v>157</v>
-      </c>
-      <c r="D75" s="7">
-        <v>77</v>
-      </c>
-      <c r="E75" s="7">
-        <v>92</v>
-      </c>
-      <c r="F75" s="7">
-        <v>107</v>
-      </c>
-      <c r="G75" s="7">
-        <v>103</v>
-      </c>
-      <c r="H75" s="7">
-        <v>141</v>
-      </c>
-      <c r="I75" s="7">
-        <v>167</v>
-      </c>
-      <c r="J75" s="7">
-        <v>160</v>
-      </c>
-      <c r="K75" s="7">
-        <v>162</v>
+        <v>8708</v>
+      </c>
+      <c r="C75" s="2">
+        <v>158</v>
+      </c>
+      <c r="D75" s="2">
+        <v>102</v>
+      </c>
+      <c r="E75" s="2">
+        <v>80</v>
+      </c>
+      <c r="F75" s="2">
+        <v>59</v>
+      </c>
+      <c r="G75" s="2">
+        <v>40</v>
+      </c>
+      <c r="H75" s="2">
+        <v>40</v>
+      </c>
+      <c r="I75" s="2">
+        <v>63</v>
+      </c>
+      <c r="J75" s="2">
+        <v>89</v>
+      </c>
+      <c r="K75" s="2">
+        <v>102</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B76" s="1">
-        <v>8348</v>
-      </c>
-      <c r="C76" s="7">
-        <v>139</v>
-      </c>
-      <c r="D76" s="7">
-        <v>153</v>
-      </c>
-      <c r="E76" s="7">
-        <v>151</v>
-      </c>
-      <c r="F76" s="7">
-        <v>159</v>
-      </c>
-      <c r="G76" s="7">
-        <v>141</v>
-      </c>
-      <c r="H76" s="7">
-        <v>142</v>
-      </c>
-      <c r="I76" s="7">
-        <v>148</v>
-      </c>
-      <c r="J76" s="7">
-        <v>161</v>
-      </c>
-      <c r="K76" s="7">
-        <v>152</v>
+        <v>8709</v>
+      </c>
+      <c r="C76" s="2">
+        <v>138</v>
+      </c>
+      <c r="D76" s="2">
+        <v>91</v>
+      </c>
+      <c r="E76" s="2">
+        <v>98</v>
+      </c>
+      <c r="F76" s="2">
+        <v>85</v>
+      </c>
+      <c r="G76" s="2">
+        <v>76</v>
+      </c>
+      <c r="H76" s="2">
+        <v>67</v>
+      </c>
+      <c r="I76" s="2">
+        <v>85</v>
+      </c>
+      <c r="J76" s="2">
+        <v>91</v>
+      </c>
+      <c r="K76" s="2">
+        <v>102</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B77" s="1">
-        <v>8789</v>
-      </c>
-      <c r="C77" s="7">
-        <v>138</v>
-      </c>
-      <c r="D77" s="7">
-        <v>154</v>
-      </c>
-      <c r="E77" s="7">
-        <v>117</v>
-      </c>
-      <c r="F77" s="7">
-        <v>64</v>
-      </c>
-      <c r="G77" s="7">
-        <v>56</v>
-      </c>
-      <c r="H77" s="7">
-        <v>61</v>
-      </c>
-      <c r="I77" s="7">
-        <v>68</v>
-      </c>
-      <c r="J77" s="7">
-        <v>90</v>
-      </c>
-      <c r="K77" s="7">
-        <v>81</v>
+        <v>8710</v>
+      </c>
+      <c r="C77" s="2">
+        <v>131</v>
+      </c>
+      <c r="D77" s="2">
+        <v>91</v>
+      </c>
+      <c r="E77" s="2">
+        <v>53</v>
+      </c>
+      <c r="F77" s="2">
+        <v>34</v>
+      </c>
+      <c r="G77" s="2">
+        <v>32</v>
+      </c>
+      <c r="H77" s="2">
+        <v>28</v>
+      </c>
+      <c r="I77" s="2">
+        <v>43</v>
+      </c>
+      <c r="J77" s="2">
+        <v>77</v>
+      </c>
+      <c r="K77" s="2">
+        <v>101</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B78" s="1">
-        <v>8790</v>
-      </c>
-      <c r="C78" s="7">
-        <v>128</v>
-      </c>
-      <c r="D78" s="7">
-        <v>101</v>
-      </c>
-      <c r="E78" s="7">
-        <v>98</v>
-      </c>
-      <c r="F78" s="7">
-        <v>113</v>
-      </c>
-      <c r="G78" s="7">
-        <v>113</v>
-      </c>
-      <c r="H78" s="7">
-        <v>129</v>
-      </c>
-      <c r="I78" s="7">
-        <v>153</v>
-      </c>
-      <c r="J78" s="7">
-        <v>173</v>
-      </c>
-      <c r="K78" s="7">
-        <v>180</v>
+        <v>8711</v>
+      </c>
+      <c r="C78" s="2">
+        <v>162</v>
+      </c>
+      <c r="D78" s="2">
+        <v>89</v>
+      </c>
+      <c r="E78" s="2">
+        <v>49</v>
+      </c>
+      <c r="F78" s="2">
+        <v>28</v>
+      </c>
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+      <c r="I78" s="2"/>
+      <c r="J78" s="2"/>
+      <c r="K78" s="2"/>
+      <c r="L78" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B79" s="1">
+        <v>8712</v>
+      </c>
+      <c r="C79" s="2">
+        <v>158</v>
+      </c>
+      <c r="D79" s="2">
+        <v>113</v>
+      </c>
+      <c r="E79" s="2">
+        <v>92</v>
+      </c>
+      <c r="F79" s="2">
+        <v>85</v>
+      </c>
+      <c r="G79" s="2">
+        <v>66</v>
+      </c>
+      <c r="H79" s="2">
+        <v>63</v>
+      </c>
+      <c r="I79" s="2">
+        <v>78</v>
+      </c>
+      <c r="J79" s="2">
+        <v>92</v>
+      </c>
+      <c r="K79" s="2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
+      <c r="J80" s="2"/>
+      <c r="K80" s="2"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+      <c r="I81" s="2"/>
+      <c r="J81" s="2"/>
+      <c r="K81" s="2"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+      <c r="H82" s="2"/>
+      <c r="I82" s="2"/>
+      <c r="J82" s="2"/>
+      <c r="K82" s="2"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B83" s="1">
+        <v>8151</v>
+      </c>
+      <c r="C83" s="2">
+        <v>165</v>
+      </c>
+      <c r="D83" s="2">
+        <v>131</v>
+      </c>
+      <c r="E83" s="2">
+        <v>102</v>
+      </c>
+      <c r="F83" s="2">
+        <v>84</v>
+      </c>
+      <c r="G83" s="2">
+        <v>91</v>
+      </c>
+      <c r="H83" s="2">
+        <v>103</v>
+      </c>
+      <c r="I83" s="2">
+        <v>143</v>
+      </c>
+      <c r="J83" s="2">
+        <v>158</v>
+      </c>
+      <c r="K83" s="2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B84" s="1">
+        <v>8152</v>
+      </c>
+      <c r="C84" s="2">
+        <v>173</v>
+      </c>
+      <c r="D84" s="2">
+        <v>137</v>
+      </c>
+      <c r="E84" s="2">
+        <v>102</v>
+      </c>
+      <c r="F84" s="2">
+        <v>105</v>
+      </c>
+      <c r="G84" s="2">
+        <v>131</v>
+      </c>
+      <c r="H84" s="2">
+        <v>195</v>
+      </c>
+      <c r="I84" s="2">
+        <v>223</v>
+      </c>
+      <c r="J84" s="2">
+        <v>227</v>
+      </c>
+      <c r="K84" s="2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B85" s="1">
+        <v>8153</v>
+      </c>
+      <c r="C85" s="2">
+        <v>194</v>
+      </c>
+      <c r="D85" s="2">
+        <v>193</v>
+      </c>
+      <c r="E85" s="2">
+        <v>93</v>
+      </c>
+      <c r="F85" s="2">
+        <v>92</v>
+      </c>
+      <c r="G85" s="2">
+        <v>103</v>
+      </c>
+      <c r="H85" s="2">
+        <v>131</v>
+      </c>
+      <c r="I85" s="2">
+        <v>159</v>
+      </c>
+      <c r="J85" s="2">
+        <v>176</v>
+      </c>
+      <c r="K85" s="2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B86" s="1">
+        <v>8154</v>
+      </c>
+      <c r="C86" s="2">
+        <v>165</v>
+      </c>
+      <c r="D86" s="2">
+        <v>128</v>
+      </c>
+      <c r="E86" s="2">
+        <v>92</v>
+      </c>
+      <c r="F86" s="2">
+        <v>80</v>
+      </c>
+      <c r="G86" s="2">
+        <v>112</v>
+      </c>
+      <c r="H86" s="2">
+        <v>142</v>
+      </c>
+      <c r="I86" s="2">
+        <v>155</v>
+      </c>
+      <c r="J86" s="2">
+        <v>192</v>
+      </c>
+      <c r="K86" s="2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B87" s="1">
+        <v>8827</v>
+      </c>
+      <c r="C87" s="6">
+        <v>147</v>
+      </c>
+      <c r="D87" s="6">
+        <v>107</v>
+      </c>
+      <c r="E87" s="6">
+        <v>92</v>
+      </c>
+      <c r="F87" s="6">
+        <v>98</v>
+      </c>
+      <c r="G87" s="6">
+        <v>114</v>
+      </c>
+      <c r="H87" s="6">
+        <v>140</v>
+      </c>
+      <c r="I87" s="6">
+        <v>174</v>
+      </c>
+      <c r="J87" s="6">
+        <v>179</v>
+      </c>
+      <c r="K87" s="6">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B88" s="1">
+        <v>8828</v>
+      </c>
+      <c r="C88" s="6">
+        <v>122</v>
+      </c>
+      <c r="D88" s="6">
+        <v>71</v>
+      </c>
+      <c r="E88" s="6">
+        <v>91</v>
+      </c>
+      <c r="F88" s="6">
+        <v>86</v>
+      </c>
+      <c r="G88" s="6">
+        <v>118</v>
+      </c>
+      <c r="H88" s="6">
+        <v>136</v>
+      </c>
+      <c r="I88" s="6">
+        <v>182</v>
+      </c>
+      <c r="J88" s="6">
+        <v>219</v>
+      </c>
+      <c r="K88" s="6">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B89" s="1">
+        <v>8829</v>
+      </c>
+      <c r="C89" s="2">
+        <v>166</v>
+      </c>
+      <c r="D89" s="2">
+        <v>150</v>
+      </c>
+      <c r="E89" s="2">
+        <v>103</v>
+      </c>
+      <c r="F89" s="2">
+        <v>107</v>
+      </c>
+      <c r="G89" s="2">
+        <v>113</v>
+      </c>
+      <c r="H89" s="2">
+        <v>146</v>
+      </c>
+      <c r="I89" s="2">
+        <v>183</v>
+      </c>
+      <c r="J89" s="2">
+        <v>196</v>
+      </c>
+      <c r="K89" s="2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B90" s="1">
+        <v>861</v>
+      </c>
+      <c r="C90" s="2">
+        <v>237</v>
+      </c>
+      <c r="D90" s="2">
+        <v>235</v>
+      </c>
+      <c r="E90" s="2">
+        <v>121</v>
+      </c>
+      <c r="F90" s="2">
+        <v>128</v>
+      </c>
+      <c r="G90" s="2">
+        <v>165</v>
+      </c>
+      <c r="H90" s="2">
+        <v>209</v>
+      </c>
+      <c r="I90" s="2">
+        <v>208</v>
+      </c>
+      <c r="J90" s="2">
+        <v>196</v>
+      </c>
+      <c r="K90" s="2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B91" s="1">
+        <v>887</v>
+      </c>
+      <c r="C91" s="2">
+        <v>132</v>
+      </c>
+      <c r="D91" s="2">
+        <v>137</v>
+      </c>
+      <c r="E91" s="2">
+        <v>124</v>
+      </c>
+      <c r="F91" s="2">
+        <v>91</v>
+      </c>
+      <c r="G91" s="2">
+        <v>136</v>
+      </c>
+      <c r="H91" s="2">
+        <v>172</v>
+      </c>
+      <c r="I91" s="2">
+        <v>174</v>
+      </c>
+      <c r="J91" s="2">
+        <v>186</v>
+      </c>
+      <c r="K91" s="2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A93" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B93" s="7">
+        <v>8560</v>
+      </c>
+      <c r="C93" s="7">
+        <v>196</v>
+      </c>
+      <c r="D93" s="7">
+        <v>124</v>
+      </c>
+      <c r="E93" s="7">
+        <v>151</v>
+      </c>
+      <c r="F93" s="7">
+        <v>155</v>
+      </c>
+      <c r="G93" s="7">
+        <v>148</v>
+      </c>
+      <c r="H93" s="7">
+        <v>151</v>
+      </c>
+      <c r="I93" s="7">
+        <v>153</v>
+      </c>
+      <c r="J93" s="7">
+        <v>168</v>
+      </c>
+      <c r="K93" s="7">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B94" s="1">
+        <v>8347</v>
+      </c>
+      <c r="C94" s="7">
+        <v>157</v>
+      </c>
+      <c r="D94" s="7">
+        <v>77</v>
+      </c>
+      <c r="E94" s="7">
+        <v>92</v>
+      </c>
+      <c r="F94" s="7">
+        <v>107</v>
+      </c>
+      <c r="G94" s="7">
+        <v>103</v>
+      </c>
+      <c r="H94" s="7">
+        <v>141</v>
+      </c>
+      <c r="I94" s="7">
+        <v>167</v>
+      </c>
+      <c r="J94" s="7">
+        <v>160</v>
+      </c>
+      <c r="K94" s="7">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B95" s="1">
+        <v>8348</v>
+      </c>
+      <c r="C95" s="7">
+        <v>139</v>
+      </c>
+      <c r="D95" s="7">
+        <v>153</v>
+      </c>
+      <c r="E95" s="7">
+        <v>151</v>
+      </c>
+      <c r="F95" s="7">
+        <v>159</v>
+      </c>
+      <c r="G95" s="7">
+        <v>141</v>
+      </c>
+      <c r="H95" s="7">
+        <v>142</v>
+      </c>
+      <c r="I95" s="7">
+        <v>148</v>
+      </c>
+      <c r="J95" s="7">
+        <v>161</v>
+      </c>
+      <c r="K95" s="7">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B96" s="1">
+        <v>8789</v>
+      </c>
+      <c r="C96" s="7">
+        <v>138</v>
+      </c>
+      <c r="D96" s="7">
+        <v>154</v>
+      </c>
+      <c r="E96" s="7">
+        <v>117</v>
+      </c>
+      <c r="F96" s="7">
+        <v>64</v>
+      </c>
+      <c r="G96" s="7">
+        <v>56</v>
+      </c>
+      <c r="H96" s="7">
+        <v>61</v>
+      </c>
+      <c r="I96" s="7">
+        <v>68</v>
+      </c>
+      <c r="J96" s="7">
+        <v>90</v>
+      </c>
+      <c r="K96" s="7">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B97" s="1">
+        <v>8790</v>
+      </c>
+      <c r="C97" s="7">
+        <v>128</v>
+      </c>
+      <c r="D97" s="7">
+        <v>101</v>
+      </c>
+      <c r="E97" s="7">
+        <v>98</v>
+      </c>
+      <c r="F97" s="7">
+        <v>113</v>
+      </c>
+      <c r="G97" s="7">
+        <v>113</v>
+      </c>
+      <c r="H97" s="7">
+        <v>129</v>
+      </c>
+      <c r="I97" s="7">
+        <v>153</v>
+      </c>
+      <c r="J97" s="7">
+        <v>173</v>
+      </c>
+      <c r="K97" s="7">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B98" s="1">
         <v>8832</v>
       </c>
-      <c r="C79" s="7">
+      <c r="C98" s="7">
         <v>115</v>
       </c>
-      <c r="D79" s="7">
+      <c r="D98" s="7">
         <v>112</v>
       </c>
-      <c r="E79" s="7">
+      <c r="E98" s="7">
         <v>90</v>
       </c>
-      <c r="F79" s="7">
+      <c r="F98" s="7">
         <v>103</v>
       </c>
-      <c r="G79" s="7">
+      <c r="G98" s="7">
         <v>102</v>
       </c>
-      <c r="H79" s="7">
+      <c r="H98" s="7">
         <v>96</v>
       </c>
-      <c r="I79" s="7">
+      <c r="I98" s="7">
         <v>101</v>
       </c>
-      <c r="J79" s="7">
+      <c r="J98" s="7">
         <v>107</v>
       </c>
-      <c r="K79" s="7">
+      <c r="K98" s="7">
         <v>120</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B99" s="1">
         <v>8833</v>
       </c>
-      <c r="C80" s="7">
+      <c r="C99" s="7">
         <v>134</v>
       </c>
-      <c r="D80" s="6">
+      <c r="D99" s="6">
         <v>94</v>
       </c>
-      <c r="E80" s="6">
+      <c r="E99" s="6">
         <v>87</v>
       </c>
-      <c r="F80" s="6">
+      <c r="F99" s="6">
         <v>93</v>
       </c>
-      <c r="G80" s="6">
+      <c r="G99" s="6">
         <v>116</v>
       </c>
-      <c r="H80" s="6">
+      <c r="H99" s="6">
         <v>128</v>
       </c>
-      <c r="I80" s="6">
+      <c r="I99" s="6">
         <v>123</v>
       </c>
-      <c r="J80" s="6">
+      <c r="J99" s="6">
         <v>136</v>
       </c>
-      <c r="K80" s="6">
+      <c r="K99" s="6">
         <v>135</v>
       </c>
-      <c r="L80" s="6"/>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
+      <c r="L99" s="6"/>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B81" s="1">
+      <c r="B100" s="1">
         <v>8834</v>
       </c>
-      <c r="C81" s="7">
+      <c r="C100" s="7">
         <v>111</v>
       </c>
-      <c r="D81" s="7">
+      <c r="D100" s="7">
         <v>82</v>
       </c>
-      <c r="E81" s="7">
+      <c r="E100" s="7">
         <v>75</v>
       </c>
-      <c r="F81" s="7">
+      <c r="F100" s="7">
         <v>82</v>
       </c>
-      <c r="G81" s="7">
+      <c r="G100" s="7">
         <v>97</v>
       </c>
-      <c r="H81" s="7">
+      <c r="H100" s="7">
         <v>107</v>
       </c>
-      <c r="I81" s="7">
+      <c r="I100" s="7">
         <v>118</v>
       </c>
-      <c r="J81" s="7">
+      <c r="J100" s="7">
         <v>117</v>
       </c>
-      <c r="K81" s="7">
+      <c r="K100" s="7">
         <v>108</v>
       </c>
     </row>
@@ -3055,7 +3775,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA59B8A1-7D09-714E-A404-B72F68DCA331}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>